<commit_message>
update for auto install M
</commit_message>
<xml_diff>
--- a/inst/extdata/james-local-settings.xlsx
+++ b/inst/extdata/james-local-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D003D-F815-5744-AE09-2D816E78C547}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF96462-EA97-CF4F-B3FC-CC225DD22AC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12880" yWindow="2260" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -813,9 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Fixes + new functionality for exporting data file
</commit_message>
<xml_diff>
--- a/inst/extdata/james-local-settings.xlsx
+++ b/inst/extdata/james-local-settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF96462-EA97-CF4F-B3FC-CC225DD22AC6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA028C28-EFC0-474F-814A-0E83F4DBC11B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="2260" windowWidth="19200" windowHeight="17540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
   <sheets>
     <sheet name="base_settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="148">
   <si>
     <t>decimal_sep</t>
   </si>
@@ -237,12 +237,6 @@
     <t>legend_distance_columns</t>
   </si>
   <si>
-    <t>number of whitespaces</t>
-  </si>
-  <si>
-    <t>number of whitespaces added to each of the series names &lt;may be tricky&gt;</t>
-  </si>
-  <si>
     <t>degrees</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>number of columsn in legend (empty: let James determine)</t>
   </si>
   <si>
-    <t>#0071bb, #7dcef1, #ed0579, #fbd4dc, #95817b, #00aeef, #003f71, #7b0052</t>
-  </si>
-  <si>
     <t>background color</t>
   </si>
   <si>
@@ -375,9 +366,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>James creates figures only if this value is: y, yes, Yes, or Y</t>
-  </si>
-  <si>
     <t>col_default</t>
   </si>
   <si>
@@ -433,6 +421,54 @@
   </si>
   <si>
     <t>relative size of legend text (default is 1)</t>
+  </si>
+  <si>
+    <t>number of whitespaces added to each of the series names</t>
+  </si>
+  <si>
+    <t>number of whitespaces &lt;may be tricky&gt;</t>
+  </si>
+  <si>
+    <t>legend_show</t>
+  </si>
+  <si>
+    <t>James shows legend if and only if this value is y, yes, Yes, or Y</t>
+  </si>
+  <si>
+    <t>James creates figures if and only if this value is y, yes, Yes, or Y</t>
+  </si>
+  <si>
+    <t>publish</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Indicates whether figure is to be published</t>
+  </si>
+  <si>
+    <t># PIES</t>
+  </si>
+  <si>
+    <t>pie_radius</t>
+  </si>
+  <si>
+    <t>pie_show_value</t>
+  </si>
+  <si>
+    <t>pie_donut</t>
+  </si>
+  <si>
+    <t>donut_radius</t>
+  </si>
+  <si>
+    <t>#0071bb, #7dcef1, #ed0579, #fbd4dc, #95817b, #00aeef, #003f71, #7b0052, #F0E68C</t>
+  </si>
+  <si>
+    <t>col_shading</t>
+  </si>
+  <si>
+    <t>#ed057933</t>
   </si>
 </sst>
 </file>
@@ -811,14 +847,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -838,211 +876,206 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B4" t="s">
-        <v>123</v>
-      </c>
+      <c r="B4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
-    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>117</v>
+      <c r="A9" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>126</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22">
-        <v>1.3</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>2</v>
@@ -1050,481 +1083,554 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
       <c r="D25" s="3" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>64</v>
       </c>
-      <c r="B28">
+      <c r="B30">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33">
+        <v>0.02</v>
+      </c>
+      <c r="C33" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B31">
-        <v>0.02</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34">
-        <v>1.5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>0.25</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B36">
-        <v>0.25</v>
+        <v>1.5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>1</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>30</v>
       </c>
-      <c r="B41">
+      <c r="B43">
         <v>0.4</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46">
+        <v>0.4</v>
+      </c>
+      <c r="C46" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44">
-        <v>0.4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>126</v>
-      </c>
-      <c r="D47" t="s">
-        <v>72</v>
-      </c>
-    </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48">
-        <v>-0.6</v>
-      </c>
-      <c r="C48" t="s">
-        <v>17</v>
+      <c r="A48" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>86</v>
+      <c r="A49" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="B49">
-        <v>0.02</v>
-      </c>
-      <c r="C49" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" t="s">
-        <v>87</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50">
-        <v>0.25</v>
+        <v>142</v>
+      </c>
+      <c r="B50" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B51">
-        <v>-1.4999999999999999E-2</v>
+        <v>143</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B52">
-        <v>0.9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>133</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>3</v>
+      <c r="A55" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="B55">
-        <v>7.5</v>
+        <v>0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B56">
-        <v>7.5</v>
-      </c>
-      <c r="D56" t="s">
-        <v>4</v>
+        <v>-0.6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>0.02</v>
+      </c>
+      <c r="C57" t="s">
+        <v>85</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>21</v>
-      </c>
-      <c r="D58" t="s">
-        <v>4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>58</v>
+        <v>-1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>128</v>
+      </c>
+      <c r="B60">
+        <v>0.9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" t="s">
-        <v>83</v>
+      <c r="A62" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>134</v>
+      <c r="A63" t="s">
+        <v>3</v>
       </c>
       <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
-        <v>135</v>
+        <v>7.5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="B64">
-        <v>0.5</v>
-      </c>
-      <c r="C64" t="s">
-        <v>60</v>
+        <v>7.5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B65">
-        <v>0.5</v>
-      </c>
-      <c r="C65" t="s">
-        <v>62</v>
+        <v>21</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B66">
-        <v>2</v>
-      </c>
-      <c r="C66" t="s">
-        <v>66</v>
+        <v>21</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="B67">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73">
         <v>0.5</v>
       </c>
-      <c r="C67" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>90</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69">
-        <v>3</v>
-      </c>
-      <c r="C69" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>77</v>
-      </c>
-      <c r="B70">
-        <v>0.03</v>
-      </c>
-      <c r="C70" t="s">
-        <v>79</v>
-      </c>
-      <c r="D70" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B71">
-        <v>0.12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>45</v>
+      <c r="C73" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B74">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C74" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B75">
-        <v>0.5</v>
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B76">
         <v>0.5</v>
       </c>
+      <c r="C76" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B77">
-        <v>0.25</v>
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C78" t="s">
-        <v>46</v>
+        <v>132</v>
+      </c>
+      <c r="D78" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="B79">
-        <v>1.5</v>
+        <v>0.03</v>
+      </c>
+      <c r="C79" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="B80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>42</v>
-      </c>
-      <c r="B81">
-        <v>0</v>
+        <v>0.12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>109</v>
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83">
+        <v>0.6</v>
+      </c>
+      <c r="C83" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>112</v>
-      </c>
-      <c r="B84" t="s">
-        <v>110</v>
-      </c>
-      <c r="C84" t="s">
-        <v>113</v>
+        <v>18</v>
+      </c>
+      <c r="B84">
+        <v>0.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>111</v>
+        <v>19</v>
       </c>
       <c r="B85">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>43</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>44</v>
+      </c>
+      <c r="B88">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>41</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>109</v>
+      </c>
+      <c r="B93" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>108</v>
+      </c>
+      <c r="B94">
         <v>2400</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes, upgrades, including graphs
</commit_message>
<xml_diff>
--- a/inst/extdata/james-local-settings.xlsx
+++ b/inst/extdata/james-local-settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA028C28-EFC0-474F-814A-0E83F4DBC11B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3B89A-0A23-AB44-AAAF-533FDB27E8D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="23540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
   <sheets>
     <sheet name="base_settings" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="167">
   <si>
     <t>decimal_sep</t>
   </si>
@@ -297,15 +303,9 @@
     <t>decimal separator</t>
   </si>
   <si>
-    <t>#7dcef1, #00aeef, #003f71</t>
-  </si>
-  <si>
     <t>col_fan_line</t>
   </si>
   <si>
-    <t>#ed0579</t>
-  </si>
-  <si>
     <t>base color for fans (is dilluted)</t>
   </si>
   <si>
@@ -372,9 +372,6 @@
     <t>col_default_with_fan</t>
   </si>
   <si>
-    <t>#fbd4dc, #95817b, #003f71, #7b0052</t>
-  </si>
-  <si>
     <t>default colors when fan is used</t>
   </si>
   <si>
@@ -408,9 +405,6 @@
     <t>#ffffff</t>
   </si>
   <si>
-    <t>white, red</t>
-  </si>
-  <si>
     <t>v_shift_x_lab</t>
   </si>
   <si>
@@ -432,9 +426,6 @@
     <t>legend_show</t>
   </si>
   <si>
-    <t>James shows legend if and only if this value is y, yes, Yes, or Y</t>
-  </si>
-  <si>
     <t>James creates figures if and only if this value is y, yes, Yes, or Y</t>
   </si>
   <si>
@@ -462,13 +453,85 @@
     <t>donut_radius</t>
   </si>
   <si>
-    <t>#0071bb, #7dcef1, #ed0579, #fbd4dc, #95817b, #00aeef, #003f71, #7b0052, #F0E68C</t>
-  </si>
-  <si>
     <t>col_shading</t>
   </si>
   <si>
-    <t>#ed057933</t>
+    <t>#005faf, #87d2ff, #e6006e, #f596af, #96827d, #d7c8c8, #820050, #193c69, #64504b</t>
+  </si>
+  <si>
+    <t>#87d2ff90, #00a5eb90, #005faf99</t>
+  </si>
+  <si>
+    <t>#e6006e</t>
+  </si>
+  <si>
+    <t>#f596af, #96827d, #d7c8c8, #820050</t>
+  </si>
+  <si>
+    <t>white, #e6006e</t>
+  </si>
+  <si>
+    <t>#e6006e33</t>
+  </si>
+  <si>
+    <t>Specify n to disable legend, y to show legend or comma separated number of series you want to show</t>
+  </si>
+  <si>
+    <t>publish_data</t>
+  </si>
+  <si>
+    <t>Indicates whether figure's data is also (true if and only if both publish and publish_data are y)</t>
+  </si>
+  <si>
+    <t># GRAPH</t>
+  </si>
+  <si>
+    <t>legend_line_length_graph</t>
+  </si>
+  <si>
+    <t>length of line segment in graphs</t>
+  </si>
+  <si>
+    <t>#87d2ff</t>
+  </si>
+  <si>
+    <t>graph_edge_color</t>
+  </si>
+  <si>
+    <t>graph_node_color</t>
+  </si>
+  <si>
+    <t>graph_arrow_size</t>
+  </si>
+  <si>
+    <t>graph_node_size</t>
+  </si>
+  <si>
+    <t>size_graph</t>
+  </si>
+  <si>
+    <t>size of font in graph with nodes and edges</t>
+  </si>
+  <si>
+    <t>graph_edge_curved</t>
+  </si>
+  <si>
+    <t>graph_node_text_color</t>
+  </si>
+  <si>
+    <t>size of nodes</t>
+  </si>
+  <si>
+    <t>choose [0, 1]</t>
+  </si>
+  <si>
+    <t>graph_set_margins_to_zero</t>
+  </si>
+  <si>
+    <t>y, n</t>
+  </si>
+  <si>
+    <t>reserve more space for graph</t>
   </si>
 </sst>
 </file>
@@ -527,12 +590,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -876,762 +940,862 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>119</v>
+      <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>90</v>
+        <v>111</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" t="s">
         <v>91</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
+        <v>90</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" t="s">
-        <v>127</v>
+        <v>112</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" t="s">
-        <v>92</v>
+        <v>120</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>126</v>
+        <v>114</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>146</v>
-      </c>
-      <c r="B18" t="s">
-        <v>147</v>
+        <v>22</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
+        <v>140</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
+      <c r="A22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>1.3</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>2</v>
+        <v>155</v>
+      </c>
+      <c r="B24" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>2</v>
+      <c r="A26" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
         <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>1.3</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33">
-        <v>0.02</v>
-      </c>
-      <c r="C33" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" t="s">
-        <v>104</v>
+      <c r="A32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36">
-        <v>1.5</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
+      <c r="A35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37">
-        <v>0.25</v>
-      </c>
-      <c r="C37" t="s">
-        <v>14</v>
+      <c r="A37" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="B38">
+        <v>0.02</v>
+      </c>
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <v>1.5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>29</v>
+      <c r="C42" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>30</v>
       </c>
-      <c r="B43">
+      <c r="B48">
         <v>0.4</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C48" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46">
-        <v>0.4</v>
-      </c>
-      <c r="C46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>142</v>
-      </c>
-      <c r="B50" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>144</v>
-      </c>
-      <c r="B52">
+        <v>73</v>
+      </c>
+      <c r="B51">
         <v>0.4</v>
       </c>
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>15</v>
+      <c r="A54" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54">
+        <v>0.8</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55">
-        <v>0</v>
-      </c>
-      <c r="C55" t="s">
-        <v>122</v>
-      </c>
-      <c r="D55" t="s">
-        <v>70</v>
+      <c r="A55" t="s">
+        <v>137</v>
+      </c>
+      <c r="B55" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56">
-        <v>-0.6</v>
-      </c>
-      <c r="C56" t="s">
-        <v>17</v>
+        <v>138</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61">
+        <v>-0.6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>83</v>
       </c>
-      <c r="B57">
+      <c r="B62">
         <v>0.02</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C62" t="s">
         <v>85</v>
-      </c>
-      <c r="D57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59">
-        <v>-1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>128</v>
-      </c>
-      <c r="B60">
-        <v>0.9</v>
-      </c>
-      <c r="C60" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B63">
-        <v>7.5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B64">
-        <v>7.5</v>
-      </c>
-      <c r="D64" t="s">
-        <v>4</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="B65">
-        <v>21</v>
-      </c>
-      <c r="D65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B66">
-        <v>21</v>
-      </c>
-      <c r="D66" t="s">
-        <v>4</v>
+        <v>0.9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s">
-        <v>11</v>
+      <c r="A67" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>58</v>
+      <c r="A69" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B70" t="s">
-        <v>112</v>
+        <v>126</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>80</v>
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71">
+        <v>0.5</v>
       </c>
       <c r="C71" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>130</v>
+      <c r="A72" t="s">
+        <v>61</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B73">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>60</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B74">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C75" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B76">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>88</v>
+        <v>128</v>
+      </c>
+      <c r="D77" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="C78" t="s">
-        <v>132</v>
+        <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B79">
-        <v>0.03</v>
-      </c>
-      <c r="C79" t="s">
-        <v>77</v>
+        <v>0.12</v>
       </c>
       <c r="D79" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>76</v>
-      </c>
-      <c r="B80">
-        <v>0.12</v>
-      </c>
-      <c r="D80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>156</v>
+      </c>
+      <c r="B82">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84">
+        <v>0.3</v>
+      </c>
+      <c r="C84" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" t="s">
+        <v>110</v>
+      </c>
+      <c r="C85" t="s">
+        <v>166</v>
+      </c>
+      <c r="D85" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>7.5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>7.5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>48</v>
+      </c>
+      <c r="B90">
+        <v>21</v>
+      </c>
+      <c r="D90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91">
+        <v>21</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>21</v>
       </c>
-      <c r="B83">
+      <c r="B95">
         <v>0.6</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C95" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>18</v>
       </c>
-      <c r="B84">
+      <c r="B96">
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>19</v>
       </c>
-      <c r="B85">
+      <c r="B97">
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>20</v>
       </c>
-      <c r="B86">
+      <c r="B98">
         <v>0.25</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>43</v>
       </c>
-      <c r="B87">
+      <c r="B99">
         <v>0</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C99" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>44</v>
       </c>
-      <c r="B88">
+      <c r="B100">
         <v>1.5</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>41</v>
       </c>
-      <c r="B89">
+      <c r="B101">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>42</v>
       </c>
-      <c r="B90">
+      <c r="B102">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>109</v>
-      </c>
-      <c r="B93" t="s">
-        <v>107</v>
-      </c>
-      <c r="C93" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="B106">
+        <v>2400</v>
+      </c>
+      <c r="C106" t="s">
         <v>108</v>
-      </c>
-      <c r="B94">
-        <v>2400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates + fix igraph
</commit_message>
<xml_diff>
--- a/inst/extdata/james-local-settings.xlsx
+++ b/inst/extdata/james-local-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC3B89A-0A23-AB44-AAAF-533FDB27E8D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21C75E-FCA9-0143-91AA-C92A90B9D681}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="168">
   <si>
     <t>decimal_sep</t>
   </si>
@@ -532,6 +532,9 @@
   </si>
   <si>
     <t>reserve more space for graph</t>
+  </si>
+  <si>
+    <t>#005faf, #87d2ff, #e6006e, #f596af, #96827d, #d7c8c8, #820050, #193c69, #64504b, darkgreen</t>
   </si>
 </sst>
 </file>
@@ -913,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
   <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,7 +1025,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Many bugfixes and improvements...
</commit_message>
<xml_diff>
--- a/inst/extdata/james-local-settings.xlsx
+++ b/inst/extdata/james-local-settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21C75E-FCA9-0143-91AA-C92A90B9D681}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEB5DA-257A-9443-9E37-52A0890964BA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="172">
   <si>
     <t>decimal_sep</t>
   </si>
@@ -535,6 +535,18 @@
   </si>
   <si>
     <t>#005faf, #87d2ff, #e6006e, #f596af, #96827d, #d7c8c8, #820050, #193c69, #64504b, darkgreen</t>
+  </si>
+  <si>
+    <t>dir_svg</t>
+  </si>
+  <si>
+    <t>svg/</t>
+  </si>
+  <si>
+    <t>create_svg</t>
+  </si>
+  <si>
+    <t>Creates SVG instead of PDF and PNG</t>
   </si>
 </sst>
 </file>
@@ -914,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E64AD6-1A4D-F84C-819F-8474C164683B}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,726 +967,723 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" t="s">
-        <v>110</v>
+        <v>132</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>95</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>122</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>146</v>
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
+        <v>140</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>155</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28">
-        <v>1.3</v>
-      </c>
-      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>1.3</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>26</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="B35">
+      <c r="B37">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>101</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>0.02</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C40" t="s">
         <v>103</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41">
-        <v>1.5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42">
-        <v>0.25</v>
-      </c>
-      <c r="C42" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B43">
-        <v>0.25</v>
+        <v>1.5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>53</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>1</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>30</v>
       </c>
-      <c r="B48">
+      <c r="B50">
         <v>0.4</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>73</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>0.4</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>0.8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>137</v>
-      </c>
-      <c r="B55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>139</v>
       </c>
-      <c r="B57">
+      <c r="B59">
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <v>0</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C62" t="s">
         <v>119</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D62" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61">
-        <v>-0.6</v>
-      </c>
-      <c r="C61" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>83</v>
-      </c>
-      <c r="B62">
-        <v>0.02</v>
-      </c>
-      <c r="C62" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B63">
-        <v>0.25</v>
+        <v>-0.6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B64">
-        <v>-1.4999999999999999E-2</v>
+        <v>0.02</v>
+      </c>
+      <c r="C64" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>56</v>
+      </c>
+      <c r="B65">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>124</v>
       </c>
-      <c r="B65">
+      <c r="B67">
         <v>0.9</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C67" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B68" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C69" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B70">
+      <c r="B72">
         <v>1</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71">
-        <v>0.5</v>
-      </c>
-      <c r="C71" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>61</v>
-      </c>
-      <c r="B72">
-        <v>0.5</v>
-      </c>
-      <c r="C72" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>59</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C74" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="B75">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
-      </c>
-      <c r="D77" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="B78">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>77</v>
-      </c>
-      <c r="D78" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79" t="s">
+        <v>128</v>
+      </c>
+      <c r="D79" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>75</v>
+      </c>
+      <c r="B80">
+        <v>0.03</v>
+      </c>
+      <c r="C80" t="s">
+        <v>77</v>
+      </c>
+      <c r="D80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>76</v>
       </c>
-      <c r="B79">
+      <c r="B81">
         <v>0.12</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>156</v>
-      </c>
-      <c r="B82">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>157</v>
-      </c>
-      <c r="B83">
-        <v>20</v>
-      </c>
-      <c r="C83" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B84">
-        <v>0.3</v>
-      </c>
-      <c r="C84" t="s">
-        <v>163</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>160</v>
+      </c>
+      <c r="B86">
+        <v>0.3</v>
+      </c>
+      <c r="C86" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>164</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>110</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>166</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D87" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88">
-        <v>7.5</v>
-      </c>
-      <c r="D88" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>5</v>
-      </c>
-      <c r="B89">
-        <v>7.5</v>
-      </c>
-      <c r="D89" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="B90">
-        <v>21</v>
+        <v>7.5</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
@@ -1682,10 +1691,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B91">
-        <v>21</v>
+        <v>7.5</v>
       </c>
       <c r="D91" t="s">
         <v>4</v>
@@ -1693,111 +1702,133 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>48</v>
+      </c>
+      <c r="B92">
+        <v>21</v>
+      </c>
+      <c r="D92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93">
+        <v>21</v>
+      </c>
+      <c r="D93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>10</v>
       </c>
-      <c r="B92">
+      <c r="B94">
         <v>7</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C94" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>21</v>
-      </c>
-      <c r="B95">
-        <v>0.6</v>
-      </c>
-      <c r="C95" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>18</v>
-      </c>
-      <c r="B96">
-        <v>0.5</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B97">
-        <v>0.5</v>
+        <v>0.6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B98">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B99">
-        <v>0</v>
-      </c>
-      <c r="C99" t="s">
-        <v>46</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B100">
-        <v>1.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>42</v>
       </c>
-      <c r="B102">
+      <c r="B104">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="1" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>107</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B106">
+      <c r="B108">
         <v>2400</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C108" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added meta lty to legend
</commit_message>
<xml_diff>
--- a/inst/extdata/james-local-settings.xlsx
+++ b/inst/extdata/james-local-settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/james-package/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB20B24-3BD1-BC4A-81C0-A6C241A36F86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4894167C-F9FC-F146-B790-3C46465BD424}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{F3167BBA-F291-F644-823E-C003F64C6F84}"/>
   </bookViews>
@@ -953,7 +953,7 @@
   <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1866,7 +1866,7 @@
         <v>176</v>
       </c>
       <c r="B111" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>